<commit_message>
Refactor PopupDialog and add test stubs
</commit_message>
<xml_diff>
--- a/範例.xlsx
+++ b/範例.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\py\BaiLeHui_PanicButton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35329E42-66EC-4D40-BB85-DC4D871127A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1C3465-4627-4C94-8791-0E70B803C764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{F5F8CECC-7E8B-4260-B4FC-692C67FF9897}"/>
   </bookViews>
@@ -154,11 +154,6 @@
 壓扣</t>
   </si>
   <si>
-    <t>311客房
-壓扣</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>312客房
 壓扣</t>
   </si>
@@ -276,6 +271,10 @@
   <si>
     <t>秒</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>313客房
+壓扣</t>
   </si>
 </sst>
 </file>
@@ -918,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0302E5B4-BFEF-4815-8421-457466FD6B85}">
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.45"/>
@@ -936,7 +935,7 @@
   <sheetData>
     <row r="1" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="2:14" ht="16.899999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -1049,7 +1048,7 @@
     <row r="7" spans="2:14" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="3"/>
       <c r="C7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="e" vm="1">
         <v>#VALUE!</v>
@@ -1077,7 +1076,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N7" s="4"/>
     </row>
@@ -1113,7 +1112,7 @@
         <v>16</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -1165,22 +1164,22 @@
       <c r="B12" s="3"/>
       <c r="C12" s="9"/>
       <c r="D12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -1191,7 +1190,7 @@
     <row r="13" spans="2:14" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="3"/>
       <c r="C13" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="e" vm="1">
         <v>#VALUE!</v>
@@ -1236,22 +1235,22 @@
       <c r="B15" s="3"/>
       <c r="C15" s="9"/>
       <c r="D15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="G15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="H15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="I15" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -1305,22 +1304,22 @@
       <c r="B18" s="3"/>
       <c r="C18" s="9"/>
       <c r="D18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="6" t="s">
@@ -1335,7 +1334,7 @@
     <row r="19" spans="2:14" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="3"/>
       <c r="C19" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="2" t="e" vm="1">
         <v>#VALUE!</v>
@@ -1363,7 +1362,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N19" s="4"/>
     </row>
@@ -1385,7 +1384,7 @@
     <row r="21" spans="2:14" ht="10.050000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
@@ -1397,7 +1396,7 @@
     <row r="24" spans="2:14" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C24" s="3"/>
       <c r="D24" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="9" t="e" vm="2">
         <v>#VALUE!</v>
@@ -1413,13 +1412,13 @@
     <row r="26" spans="2:14" ht="25.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C26" s="3"/>
       <c r="D26" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E26" s="16">
         <v>0</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
@@ -1431,7 +1430,7 @@
     <row r="28" spans="2:14" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C28" s="3"/>
       <c r="D28" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" s="9" t="e" vm="3">
         <v>#VALUE!</v>

</xml_diff>